<commit_message>
Uploader fixes for optional discriminator values.
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_child_mortality_uploader/indigenous_child_mortality.xlsx
+++ b/dashboard_loader/indigenous_child_mortality_uploader/indigenous_child_mortality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -397,15 +397,13 @@
   </sheetPr>
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,9 +1469,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,15 +1698,13 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>